<commit_message>
update for new biosteam equipment lifetime feature
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/animal_bedding/_humbird2011.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/animal_bedding/_humbird2011.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yrc2\OneDrive\Code\Bioindustrial-Park\BioSTEAM 2.x.x\biorefineries\cornstover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/animal_bedding/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_93738BBF658B224CE52DD40E9AAED54DBB468F57" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DF65FEA0-AF7E-4B6D-81DA-EF033EB6C7C8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="25824" windowHeight="14016"/>
+    <workbookView xWindow="0" yWindow="2820" windowWidth="20532" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="51">
   <si>
     <t>CEPCI</t>
   </si>
@@ -182,12 +186,15 @@
   </si>
   <si>
     <t>Bag unloader</t>
+  </si>
+  <si>
+    <t>Lifetime (yr)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -246,7 +253,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -320,6 +327,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,12 +654,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM9" sqref="AM9"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,10 +697,10 @@
       <c r="B1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="6" t="s">
         <v>19</v>
       </c>
@@ -700,27 +710,27 @@
       <c r="G1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28" t="s">
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="28"/>
+      <c r="O1" s="29"/>
       <c r="P1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="Q1" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="28"/>
+      <c r="R1" s="29"/>
       <c r="S1" s="6" t="s">
         <v>37</v>
       </c>
@@ -736,37 +746,37 @@
       <c r="W1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="X1" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
       <c r="AA1" s="15" t="s">
         <v>42</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="29" t="s">
+      <c r="AC1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="28" t="s">
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28" t="s">
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28" t="s">
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="28"/>
+      <c r="AN1" s="29"/>
       <c r="AP1" s="26"/>
     </row>
     <row r="2" spans="1:42" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -2137,6 +2147,128 @@
         <v>0</v>
       </c>
       <c r="AN12" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="T13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="U13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="V13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="W13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="X13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2177,7 +2309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2194,7 +2326,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>